<commit_message>
sc: improve import tests for text, background, border theme colors
Change-Id: Icdc658e47c0e4fe20b2b38897d31278f058a6a75
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/153783
Tested-by: Jenkins
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/Test_ThemeColor_Text_Background_Border.xlsx
+++ b/sc/qa/unit/data/xlsx/Test_ThemeColor_Text_Background_Border.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\quikee\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E45258-6768-4809-87FE-D11AF147FEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F62FCD8-1619-4CAE-AF14-E29FB8706EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="14026" xr2:uid="{A5104846-C21F-430A-A747-5DB0B85FF979}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>A1</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>B3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
 </sst>
 </file>
@@ -114,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -126,26 +132,50 @@
       <left/>
       <right/>
       <top style="thick">
+        <color theme="8" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="8" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="8" tint="0.79998168889431442"/>
+      </left>
+      <right style="thick">
+        <color theme="8" tint="0.79998168889431442"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="8" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
         <color theme="8"/>
       </top>
-      <bottom style="thick">
-        <color theme="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,36 +492,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3525E16-91AE-422A-BFBB-3C9882849F62}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>